<commit_message>
last edit : 04.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDDAC67-785F-4EAB-8E7D-476EF62E3C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02AD0F8-1100-49DA-8F36-2CEF763ADA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1527,7 +1527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1559,6 +1559,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1877,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1924,14 +1932,14 @@
         <v>465</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 05.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02AD0F8-1100-49DA-8F36-2CEF763ADA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B343FA1B-90C3-4357-9F33-D8346528796D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1943,14 +1943,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 06.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B343FA1B-90C3-4357-9F33-D8346528796D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD305466-7E9D-499A-BD94-1E1717C88337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1954,14 +1954,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 07.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC12B930-EBFB-493C-93CC-7856B58443EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C1D1CE-0C04-4E05-94B8-B6CDAC014571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1976,14 +1976,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A11" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 08.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC40409-0121-490A-8297-0073F7D18BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37323C4B-5ECE-4D73-BDB3-E752E34B32D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1998,14 +1998,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A13" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 10.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37323C4B-5ECE-4D73-BDB3-E752E34B32D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7001FD7B-9F2D-478D-A165-36614BBC11BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2009,14 +2009,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 11.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8EBAE1-1EBD-47F6-BEF0-4A291AB8F585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF586FD-2944-4FBC-989B-A4D67E5F9312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2031,14 +2031,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A16" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 13.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C7CCD7-132B-46BC-9D20-73C04BE13E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065A414E-50FE-453B-A597-91BF0E43DA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2053,14 +2053,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 18.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05571ABD-2077-499D-8CFC-68C1B5F3FF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB42EEB-044D-4195-AE2E-F64E17ADDCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1884,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2075,14 +2075,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A20" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 19.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB42EEB-044D-4195-AE2E-F64E17ADDCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A825A325-9F68-425D-B31D-69B001FFBAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2086,14 +2086,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A21" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 20.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F1113F-ED77-43DF-BAED-F7BDE79D7BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C364788-F9CF-426B-A6B6-99329AEFE0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1551,22 +1551,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1884,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1921,245 +1921,245 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="14" customFormat="1" ht="21">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:3" s="16" customFormat="1" ht="21">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="15" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="18" customFormat="1" ht="21">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="21">
-      <c r="A27" s="5" t="s">
+      <c r="C26" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A27" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 21.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D9E663-A751-4F1D-AB01-E606F64C8B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AD2C7C-2791-4B62-9D05-B0F500905CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2181,7 +2181,7 @@
       <c r="B29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 22.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76D6A78-1A62-4F55-9C12-7960C00719F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EC72F4-7171-47D2-907B-87ECE2A7ADFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2214,7 +2214,7 @@
       <c r="B32" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 23.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF74379-FB63-462E-8101-EFF113E2E455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C486F42-8D9E-4CF2-9BA4-CF75EAD47836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2236,7 +2236,7 @@
       <c r="B34" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 24.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C486F42-8D9E-4CF2-9BA4-CF75EAD47836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96585F3-39E8-4909-BEB8-361E3BBBA47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1884,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2247,7 +2247,7 @@
       <c r="B35" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 25.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96585F3-39E8-4909-BEB8-361E3BBBA47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8032FD0B-A289-421D-886B-90BBBF133010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2258,7 +2258,7 @@
       <c r="B36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 26.08.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27375CE1-1DFF-4793-B9EB-9C1F49532234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C651C78-D5ED-4810-B299-3FB2C5A2ECD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2203,7 +2203,7 @@
       <c r="B31" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 01.09.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C651C78-D5ED-4810-B299-3FB2C5A2ECD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B78DC3-DC7D-41EB-BBE4-A8CE6D28D52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2280,7 +2280,7 @@
       <c r="B38" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 02.09.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97996350-2EB4-4837-BE3C-A612A12022AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD73272-356B-4AB3-BF2A-B47CF33ADB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2313,7 +2313,7 @@
       <c r="B41" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 04.09.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD73272-356B-4AB3-BF2A-B47CF33ADB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD04F8D3-91D1-4D31-B5EE-CE9A6A842070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1884,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2337,7 +2337,7 @@
       <c r="B44" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 05.09.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E865D54F-9BB9-47B4-9A78-24136CB7F055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCA17B0-7B8C-49BA-925D-1A92F4A920B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2359,7 +2359,7 @@
       <c r="B46" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 06.09.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCA17B0-7B8C-49BA-925D-1A92F4A920B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646BE38E-CB7C-4DC0-8F7C-F42A26B9B93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2370,7 +2370,7 @@
       <c r="B47" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 08.09.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646BE38E-CB7C-4DC0-8F7C-F42A26B9B93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B74653-3395-42ED-BAAC-4785BEC180AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2381,7 +2381,7 @@
       <c r="B48" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 09.09.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035DDF5D-4B54-4D8E-956D-E879BDBEA9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FC75EA-9254-41D4-8184-724A8DA56936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1890,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2458,7 +2458,7 @@
       <c r="B56" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last edit : 11.09.21
</commit_message>
<xml_diff>
--- a/FINAL450 .xlsx
+++ b/FINAL450 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Repositories\Lovebabbar450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FC75EA-9254-41D4-8184-724A8DA56936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5A5963-DB92-4780-B348-FE5C323FA63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1891,7 +1891,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2469,7 +2469,7 @@
       <c r="B57" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>